<commit_message>
Moving sheets variable inside while loop to be recalculated
</commit_message>
<xml_diff>
--- a/Producción y Contador.xlsx
+++ b/Producción y Contador.xlsx
@@ -157,12 +157,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.0000_);_([$$-409]* \(#,##0.0000\);_([$$-409]* &quot;-&quot;????_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="[$$-2C0A]\ #,##0.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -875,7 +877,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1033,7 +1035,6 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="20" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1086,6 +1087,8 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="167" fontId="2" fillId="2" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1314,7 +1317,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -29527,7 +29532,7 @@
   <dimension ref="A1:AJ997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -29563,7 +29568,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A1" s="96"/>
+      <c r="A1" s="95"/>
       <c r="C1" s="27" t="s">
         <v>13</v>
       </c>
@@ -29735,15 +29740,15 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
-      <c r="K3" s="98" t="s">
+      <c r="K3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
       <c r="R3" s="48">
         <f>AVERAGE(F2:R2)</f>
         <v>91.666666666666671</v>
@@ -29757,14 +29762,14 @@
       <c r="Y3" s="47"/>
       <c r="Z3" s="47"/>
       <c r="AA3" s="47"/>
-      <c r="AB3" s="98" t="s">
+      <c r="AB3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="99"/>
-      <c r="AD3" s="99"/>
-      <c r="AE3" s="99"/>
-      <c r="AF3" s="99"/>
-      <c r="AG3" s="100"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="100"/>
+      <c r="AG3" s="101"/>
       <c r="AH3" s="48" t="e">
         <f>AVERAGE(S2:AH2)</f>
         <v>#DIV/0!</v>
@@ -29965,15 +29970,15 @@
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="101" t="s">
+      <c r="K7" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="102"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="103"/>
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="104"/>
       <c r="R7" s="57" t="e">
         <f>AVERAGE(D6:R6)</f>
         <v>#DIV/0!</v>
@@ -29987,14 +29992,14 @@
       <c r="Y7" s="47"/>
       <c r="Z7" s="47"/>
       <c r="AA7" s="47"/>
-      <c r="AB7" s="98" t="s">
+      <c r="AB7" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="99"/>
-      <c r="AG7" s="100"/>
+      <c r="AC7" s="100"/>
+      <c r="AD7" s="100"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="100"/>
+      <c r="AG7" s="101"/>
       <c r="AH7" s="48" t="e">
         <f>AVERAGE(S6:AG6)</f>
         <v>#DIV/0!</v>
@@ -30195,15 +30200,15 @@
       <c r="H11" s="61"/>
       <c r="I11" s="61"/>
       <c r="J11" s="61"/>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="106"/>
+      <c r="L11" s="106"/>
+      <c r="M11" s="106"/>
+      <c r="N11" s="106"/>
+      <c r="O11" s="106"/>
+      <c r="P11" s="106"/>
+      <c r="Q11" s="107"/>
       <c r="R11" s="62" t="e">
         <f>AVERAGE(D10:R10)</f>
         <v>#DIV/0!</v>
@@ -30217,14 +30222,14 @@
       <c r="Y11" s="61"/>
       <c r="Z11" s="61"/>
       <c r="AA11" s="61"/>
-      <c r="AB11" s="104" t="s">
+      <c r="AB11" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="AC11" s="105"/>
-      <c r="AD11" s="105"/>
-      <c r="AE11" s="105"/>
-      <c r="AF11" s="105"/>
-      <c r="AG11" s="106"/>
+      <c r="AC11" s="106"/>
+      <c r="AD11" s="106"/>
+      <c r="AE11" s="106"/>
+      <c r="AF11" s="106"/>
+      <c r="AG11" s="107"/>
       <c r="AH11" s="62" t="e">
         <f>AVERAGE(S10:AH10)</f>
         <v>#DIV/0!</v>
@@ -30253,8 +30258,8 @@
       <c r="A14" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="67">
-        <v>8.2954E-2</v>
+      <c r="B14" s="97">
+        <v>7.3005E-2</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -30264,84 +30269,84 @@
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="69">
+      <c r="B15" s="68">
         <f>(B13*B14)</f>
-        <v>45.624699999999997</v>
+        <v>40.152749999999997</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="70">
+      <c r="B16" s="69">
         <f>B15/B23</f>
-        <v>1.2724815855015632E-2</v>
+        <v>1.1215413363723207E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
       <c r="A17" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="97">
+      <c r="B17" s="96">
         <v>185</v>
       </c>
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A18" s="68" t="s">
+      <c r="A18" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="69">
+      <c r="B18" s="68">
         <f>(B15*B17)</f>
-        <v>8440.5694999999996</v>
+        <v>7428.25875</v>
       </c>
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="71"/>
-      <c r="B19" s="72"/>
+      <c r="A19" s="70"/>
+      <c r="B19" s="71"/>
       <c r="E19" s="4"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="74">
+      <c r="B20" s="73">
         <v>660</v>
       </c>
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="73" t="s">
+      <c r="A21" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="75">
+      <c r="B21" s="74">
         <f>B20/(AJ2*B14)</f>
-        <v>86.795091255394553</v>
+        <v>98.62338196013971</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A22" s="71"/>
-      <c r="B22" s="72"/>
+      <c r="A22" s="70"/>
+      <c r="B22" s="71"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="76">
-        <v>3585.49</v>
+      <c r="B23" s="75">
+        <v>3580.14</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -31368,7 +31373,7 @@
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -31405,7 +31410,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="76" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="31">
@@ -31512,14 +31517,14 @@
       <c r="A2" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="78" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
       <c r="J2" s="41"/>
@@ -31565,15 +31570,15 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
-      <c r="K3" s="98" t="s">
+      <c r="K3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
       <c r="R3" s="48" t="e">
         <f>AVERAGE(D2:R2)</f>
         <v>#DIV/0!</v>
@@ -31587,14 +31592,14 @@
       <c r="Y3" s="47"/>
       <c r="Z3" s="47"/>
       <c r="AA3" s="47"/>
-      <c r="AB3" s="98" t="s">
+      <c r="AB3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="99"/>
-      <c r="AD3" s="99"/>
-      <c r="AE3" s="99"/>
-      <c r="AF3" s="99"/>
-      <c r="AG3" s="100"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="100"/>
+      <c r="AG3" s="101"/>
       <c r="AH3" s="48" t="e">
         <f>AVERAGE(S2:AH2)</f>
         <v>#DIV/0!</v>
@@ -31611,14 +31616,14 @@
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
       <c r="J4" s="47"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="47"/>
       <c r="T4" s="47"/>
       <c r="U4" s="47"/>
@@ -31628,7 +31633,7 @@
       <c r="Y4" s="47"/>
       <c r="Z4" s="47"/>
       <c r="AA4" s="47"/>
-      <c r="AB4" s="81"/>
+      <c r="AB4" s="80"/>
       <c r="AC4" s="47"/>
       <c r="AD4" s="47"/>
       <c r="AE4" s="47"/>
@@ -31726,13 +31731,13 @@
       <c r="AE5" s="52">
         <v>28</v>
       </c>
-      <c r="AF5" s="82">
+      <c r="AF5" s="81">
         <v>29</v>
       </c>
-      <c r="AG5" s="82">
+      <c r="AG5" s="81">
         <v>30</v>
       </c>
-      <c r="AH5" s="82">
+      <c r="AH5" s="81">
         <v>31</v>
       </c>
       <c r="AI5" s="43" t="s">
@@ -31795,15 +31800,15 @@
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="98" t="s">
+      <c r="K7" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="101"/>
       <c r="R7" s="48" t="e">
         <f>AVERAGE(D6:R6)</f>
         <v>#DIV/0!</v>
@@ -31817,14 +31822,14 @@
       <c r="Y7" s="47"/>
       <c r="Z7" s="47"/>
       <c r="AA7" s="47"/>
-      <c r="AB7" s="98" t="s">
+      <c r="AB7" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="99"/>
-      <c r="AG7" s="100"/>
+      <c r="AC7" s="100"/>
+      <c r="AD7" s="100"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="100"/>
+      <c r="AG7" s="101"/>
       <c r="AH7" s="48" t="e">
         <f>AVERAGE(S6:AE6)</f>
         <v>#DIV/0!</v>
@@ -31983,8 +31988,8 @@
       <c r="A10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="67">
-        <v>8.2954E-2</v>
+      <c r="B10" s="97">
+        <v>7.3005E-2</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>4</v>
@@ -32030,10 +32035,10 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="68">
         <f>(B9*B10)</f>
         <v>0</v>
       </c>
@@ -32045,15 +32050,15 @@
       <c r="H11" s="47"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
-      <c r="K11" s="98" t="s">
+      <c r="K11" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="101"/>
       <c r="R11" s="48" t="e">
         <f>AVERAGE(D10:R10)</f>
         <v>#DIV/0!</v>
@@ -32067,14 +32072,14 @@
       <c r="Y11" s="47"/>
       <c r="Z11" s="47"/>
       <c r="AA11" s="47"/>
-      <c r="AB11" s="98" t="s">
+      <c r="AB11" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC11" s="99"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="99"/>
-      <c r="AF11" s="99"/>
-      <c r="AG11" s="100"/>
+      <c r="AC11" s="100"/>
+      <c r="AD11" s="100"/>
+      <c r="AE11" s="100"/>
+      <c r="AF11" s="100"/>
+      <c r="AG11" s="101"/>
       <c r="AH11" s="48" t="e">
         <f>AVERAGE(S10:AH10)</f>
         <v>#DIV/0!</v>
@@ -32083,10 +32088,10 @@
       <c r="AJ11" s="49"/>
     </row>
     <row r="12" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="70">
+      <c r="B12" s="69">
         <f>B11/B16</f>
         <v>0</v>
       </c>
@@ -32129,7 +32134,7 @@
       <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="97">
+      <c r="B13" s="96">
         <v>185</v>
       </c>
       <c r="C13" s="50" t="s">
@@ -32225,7 +32230,7 @@
       <c r="AG13" s="52">
         <v>30</v>
       </c>
-      <c r="AH13" s="82">
+      <c r="AH13" s="81">
         <v>31</v>
       </c>
       <c r="AI13" s="43" t="s">
@@ -32236,10 +32241,10 @@
       </c>
     </row>
     <row r="14" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="69">
+      <c r="B14" s="68">
         <f>(B11*B13)</f>
         <v>0</v>
       </c>
@@ -32287,8 +32292,8 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="45"/>
       <c r="D15" s="46"/>
       <c r="E15" s="46"/>
@@ -32297,15 +32302,15 @@
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47"/>
-      <c r="K15" s="98" t="s">
+      <c r="K15" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="100"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="101"/>
       <c r="R15" s="48" t="e">
         <f>AVERAGE(D14:R14)</f>
         <v>#DIV/0!</v>
@@ -32319,14 +32324,14 @@
       <c r="Y15" s="47"/>
       <c r="Z15" s="47"/>
       <c r="AA15" s="47"/>
-      <c r="AB15" s="98" t="s">
+      <c r="AB15" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC15" s="99"/>
-      <c r="AD15" s="99"/>
-      <c r="AE15" s="99"/>
-      <c r="AF15" s="99"/>
-      <c r="AG15" s="100"/>
+      <c r="AC15" s="100"/>
+      <c r="AD15" s="100"/>
+      <c r="AE15" s="100"/>
+      <c r="AF15" s="100"/>
+      <c r="AG15" s="101"/>
       <c r="AH15" s="48" t="e">
         <f>AVERAGE(S14:AG14)</f>
         <v>#DIV/0!</v>
@@ -32335,11 +32340,11 @@
       <c r="AJ15" s="49"/>
     </row>
     <row r="16" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="76">
-        <v>3585.49</v>
+      <c r="B16" s="75">
+        <v>3580.14</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="46"/>
@@ -32533,15 +32538,15 @@
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="47"/>
-      <c r="K19" s="98" t="s">
+      <c r="K19" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="99"/>
-      <c r="M19" s="99"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="100"/>
+      <c r="P19" s="100"/>
+      <c r="Q19" s="101"/>
       <c r="R19" s="48" t="e">
         <f>AVERAGE(D18:R18)</f>
         <v>#DIV/0!</v>
@@ -32555,14 +32560,14 @@
       <c r="Y19" s="47"/>
       <c r="Z19" s="47"/>
       <c r="AA19" s="47"/>
-      <c r="AB19" s="98" t="s">
+      <c r="AB19" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC19" s="99"/>
-      <c r="AD19" s="99"/>
-      <c r="AE19" s="99"/>
-      <c r="AF19" s="99"/>
-      <c r="AG19" s="100"/>
+      <c r="AC19" s="100"/>
+      <c r="AD19" s="100"/>
+      <c r="AE19" s="100"/>
+      <c r="AF19" s="100"/>
+      <c r="AG19" s="101"/>
       <c r="AH19" s="48" t="e">
         <f>AVERAGE(S18:AG18)</f>
         <v>#DIV/0!</v>
@@ -32700,7 +32705,7 @@
       <c r="AG21" s="52">
         <v>30</v>
       </c>
-      <c r="AH21" s="82">
+      <c r="AH21" s="81">
         <v>31</v>
       </c>
       <c r="AI21" s="43" t="s">
@@ -32763,15 +32768,15 @@
       <c r="H23" s="47"/>
       <c r="I23" s="47"/>
       <c r="J23" s="47"/>
-      <c r="K23" s="98" t="s">
+      <c r="K23" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L23" s="99"/>
-      <c r="M23" s="99"/>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+      <c r="N23" s="100"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="100"/>
+      <c r="Q23" s="101"/>
       <c r="R23" s="48" t="e">
         <f>AVERAGE(D22:R22)</f>
         <v>#DIV/0!</v>
@@ -32785,14 +32790,14 @@
       <c r="Y23" s="47"/>
       <c r="Z23" s="47"/>
       <c r="AA23" s="47"/>
-      <c r="AB23" s="98" t="s">
+      <c r="AB23" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC23" s="99"/>
-      <c r="AD23" s="99"/>
-      <c r="AE23" s="99"/>
-      <c r="AF23" s="99"/>
-      <c r="AG23" s="100"/>
+      <c r="AC23" s="100"/>
+      <c r="AD23" s="100"/>
+      <c r="AE23" s="100"/>
+      <c r="AF23" s="100"/>
+      <c r="AG23" s="101"/>
       <c r="AH23" s="48" t="e">
         <f>AVERAGE(S22:AG22)</f>
         <v>#DIV/0!</v>
@@ -32993,36 +32998,36 @@
       <c r="H27" s="47"/>
       <c r="I27" s="47"/>
       <c r="J27" s="47"/>
-      <c r="K27" s="98" t="s">
+      <c r="K27" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L27" s="99"/>
-      <c r="M27" s="99"/>
-      <c r="N27" s="99"/>
-      <c r="O27" s="99"/>
-      <c r="P27" s="99"/>
-      <c r="Q27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="101"/>
       <c r="R27" s="48" t="e">
         <f>AVERAGE(D26:R26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S27" s="83"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="83"/>
-      <c r="V27" s="84"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="83"/>
       <c r="W27" s="47"/>
       <c r="X27" s="47"/>
       <c r="Y27" s="47"/>
       <c r="Z27" s="47"/>
       <c r="AA27" s="47"/>
-      <c r="AB27" s="98" t="s">
+      <c r="AB27" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC27" s="99"/>
-      <c r="AD27" s="99"/>
-      <c r="AE27" s="99"/>
-      <c r="AF27" s="99"/>
-      <c r="AG27" s="100"/>
+      <c r="AC27" s="100"/>
+      <c r="AD27" s="100"/>
+      <c r="AE27" s="100"/>
+      <c r="AF27" s="100"/>
+      <c r="AG27" s="101"/>
       <c r="AH27" s="48" t="e">
         <f>AVERAGE(S26:AH26)</f>
         <v>#DIV/0!</v>
@@ -33223,15 +33228,15 @@
       <c r="H31" s="47"/>
       <c r="I31" s="47"/>
       <c r="J31" s="47"/>
-      <c r="K31" s="98" t="s">
+      <c r="K31" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="101"/>
       <c r="R31" s="48" t="e">
         <f>AVERAGE(D30:R30)</f>
         <v>#DIV/0!</v>
@@ -33245,14 +33250,14 @@
       <c r="Y31" s="47"/>
       <c r="Z31" s="47"/>
       <c r="AA31" s="47"/>
-      <c r="AB31" s="98" t="s">
+      <c r="AB31" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC31" s="99"/>
-      <c r="AD31" s="99"/>
-      <c r="AE31" s="99"/>
-      <c r="AF31" s="99"/>
-      <c r="AG31" s="100"/>
+      <c r="AC31" s="100"/>
+      <c r="AD31" s="100"/>
+      <c r="AE31" s="100"/>
+      <c r="AF31" s="100"/>
+      <c r="AG31" s="101"/>
       <c r="AH31" s="48" t="e">
         <f>AVERAGE(S30:AH30)</f>
         <v>#DIV/0!</v>
@@ -33390,7 +33395,7 @@
       <c r="AG33" s="52">
         <v>30</v>
       </c>
-      <c r="AH33" s="82">
+      <c r="AH33" s="81">
         <v>31</v>
       </c>
       <c r="AI33" s="43" t="s">
@@ -33445,7 +33450,7 @@
       </c>
     </row>
     <row r="35" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C35" s="85"/>
+      <c r="C35" s="84"/>
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
@@ -33453,15 +33458,15 @@
       <c r="H35" s="47"/>
       <c r="I35" s="47"/>
       <c r="J35" s="47"/>
-      <c r="K35" s="98" t="s">
+      <c r="K35" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="99"/>
-      <c r="M35" s="99"/>
-      <c r="N35" s="99"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="101"/>
       <c r="R35" s="48" t="e">
         <f>AVERAGE(D34:R34)</f>
         <v>#DIV/0!</v>
@@ -33475,14 +33480,14 @@
       <c r="Y35" s="47"/>
       <c r="Z35" s="47"/>
       <c r="AA35" s="47"/>
-      <c r="AB35" s="98" t="s">
+      <c r="AB35" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC35" s="99"/>
-      <c r="AD35" s="99"/>
-      <c r="AE35" s="99"/>
-      <c r="AF35" s="99"/>
-      <c r="AG35" s="100"/>
+      <c r="AC35" s="100"/>
+      <c r="AD35" s="100"/>
+      <c r="AE35" s="100"/>
+      <c r="AF35" s="100"/>
+      <c r="AG35" s="101"/>
       <c r="AH35" s="48" t="e">
         <f>AVERAGE(S34:AG34)</f>
         <v>#DIV/0!</v>
@@ -33491,7 +33496,7 @@
       <c r="AJ35" s="49"/>
     </row>
     <row r="36" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C36" s="85"/>
+      <c r="C36" s="84"/>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
       <c r="F36" s="47"/>
@@ -33683,15 +33688,15 @@
       <c r="H39" s="47"/>
       <c r="I39" s="47"/>
       <c r="J39" s="47"/>
-      <c r="K39" s="98" t="s">
+      <c r="K39" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L39" s="99"/>
-      <c r="M39" s="99"/>
-      <c r="N39" s="99"/>
-      <c r="O39" s="99"/>
-      <c r="P39" s="99"/>
-      <c r="Q39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="100"/>
+      <c r="Q39" s="101"/>
       <c r="R39" s="48" t="e">
         <f>AVERAGE(D38:R38)</f>
         <v>#DIV/0!</v>
@@ -33705,14 +33710,14 @@
       <c r="Y39" s="47"/>
       <c r="Z39" s="47"/>
       <c r="AA39" s="47"/>
-      <c r="AB39" s="98" t="s">
+      <c r="AB39" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC39" s="99"/>
-      <c r="AD39" s="99"/>
-      <c r="AE39" s="99"/>
-      <c r="AF39" s="99"/>
-      <c r="AG39" s="100"/>
+      <c r="AC39" s="100"/>
+      <c r="AD39" s="100"/>
+      <c r="AE39" s="100"/>
+      <c r="AF39" s="100"/>
+      <c r="AG39" s="101"/>
       <c r="AH39" s="48" t="e">
         <f>AVERAGE(S38:AH38)</f>
         <v>#DIV/0!</v>
@@ -33850,7 +33855,7 @@
       <c r="AG41" s="52">
         <v>30</v>
       </c>
-      <c r="AH41" s="82">
+      <c r="AH41" s="81">
         <v>31</v>
       </c>
       <c r="AI41" s="43" t="s">
@@ -33913,15 +33918,15 @@
       <c r="H43" s="47"/>
       <c r="I43" s="47"/>
       <c r="J43" s="47"/>
-      <c r="K43" s="98" t="s">
+      <c r="K43" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L43" s="99"/>
-      <c r="M43" s="99"/>
-      <c r="N43" s="99"/>
-      <c r="O43" s="99"/>
-      <c r="P43" s="99"/>
-      <c r="Q43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="100"/>
+      <c r="Q43" s="101"/>
       <c r="R43" s="48" t="e">
         <f>AVERAGE(D42:R42)</f>
         <v>#DIV/0!</v>
@@ -33935,14 +33940,14 @@
       <c r="Y43" s="47"/>
       <c r="Z43" s="47"/>
       <c r="AA43" s="47"/>
-      <c r="AB43" s="98" t="s">
+      <c r="AB43" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC43" s="99"/>
-      <c r="AD43" s="99"/>
-      <c r="AE43" s="99"/>
-      <c r="AF43" s="99"/>
-      <c r="AG43" s="100"/>
+      <c r="AC43" s="100"/>
+      <c r="AD43" s="100"/>
+      <c r="AE43" s="100"/>
+      <c r="AF43" s="100"/>
+      <c r="AG43" s="101"/>
       <c r="AH43" s="48" t="e">
         <f>AVERAGE(S42:AG42)</f>
         <v>#DIV/0!</v>
@@ -34135,7 +34140,7 @@
       </c>
     </row>
     <row r="47" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C47" s="86"/>
+      <c r="C47" s="85"/>
       <c r="D47" s="61"/>
       <c r="E47" s="61"/>
       <c r="F47" s="61"/>
@@ -34143,15 +34148,15 @@
       <c r="H47" s="61"/>
       <c r="I47" s="61"/>
       <c r="J47" s="61"/>
-      <c r="K47" s="104" t="s">
+      <c r="K47" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="105"/>
-      <c r="M47" s="105"/>
-      <c r="N47" s="105"/>
-      <c r="O47" s="105"/>
-      <c r="P47" s="105"/>
-      <c r="Q47" s="106"/>
+      <c r="L47" s="106"/>
+      <c r="M47" s="106"/>
+      <c r="N47" s="106"/>
+      <c r="O47" s="106"/>
+      <c r="P47" s="106"/>
+      <c r="Q47" s="107"/>
       <c r="R47" s="62" t="e">
         <f>AVERAGE(D46:R46)</f>
         <v>#DIV/0!</v>
@@ -34165,14 +34170,14 @@
       <c r="Y47" s="61"/>
       <c r="Z47" s="61"/>
       <c r="AA47" s="61"/>
-      <c r="AB47" s="104" t="s">
+      <c r="AB47" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="AC47" s="105"/>
-      <c r="AD47" s="105"/>
-      <c r="AE47" s="105"/>
-      <c r="AF47" s="105"/>
-      <c r="AG47" s="106"/>
+      <c r="AC47" s="106"/>
+      <c r="AD47" s="106"/>
+      <c r="AE47" s="106"/>
+      <c r="AF47" s="106"/>
+      <c r="AG47" s="107"/>
       <c r="AH47" s="62" t="e">
         <f>AVERAGE(S46:AH46)</f>
         <v>#DIV/0!</v>
@@ -35135,6 +35140,18 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="AB3:AG3"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="AB7:AG7"/>
+    <mergeCell ref="K11:Q11"/>
+    <mergeCell ref="AB11:AG11"/>
+    <mergeCell ref="AB15:AG15"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K19:Q19"/>
+    <mergeCell ref="AB19:AG19"/>
+    <mergeCell ref="K23:Q23"/>
+    <mergeCell ref="AB23:AG23"/>
     <mergeCell ref="K27:Q27"/>
     <mergeCell ref="AB27:AG27"/>
     <mergeCell ref="K43:Q43"/>
@@ -35147,18 +35164,6 @@
     <mergeCell ref="K39:Q39"/>
     <mergeCell ref="AB39:AG39"/>
     <mergeCell ref="AB43:AG43"/>
-    <mergeCell ref="AB15:AG15"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="K19:Q19"/>
-    <mergeCell ref="AB19:AG19"/>
-    <mergeCell ref="K23:Q23"/>
-    <mergeCell ref="AB23:AG23"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="AB3:AG3"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="AB7:AG7"/>
-    <mergeCell ref="K11:Q11"/>
-    <mergeCell ref="AB11:AG11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -35170,7 +35175,7 @@
   <dimension ref="A1:AJ997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -35207,106 +35212,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="88">
+      <c r="D1" s="87">
         <v>1</v>
       </c>
-      <c r="E1" s="88">
+      <c r="E1" s="87">
         <v>2</v>
       </c>
-      <c r="F1" s="89">
+      <c r="F1" s="88">
         <v>3</v>
       </c>
-      <c r="G1" s="88">
+      <c r="G1" s="87">
         <v>4</v>
       </c>
-      <c r="H1" s="88">
+      <c r="H1" s="87">
         <v>5</v>
       </c>
-      <c r="I1" s="88">
+      <c r="I1" s="87">
         <v>6</v>
       </c>
-      <c r="J1" s="88">
+      <c r="J1" s="87">
         <v>7</v>
       </c>
-      <c r="K1" s="88">
+      <c r="K1" s="87">
         <v>8</v>
       </c>
-      <c r="L1" s="88">
+      <c r="L1" s="87">
         <v>9</v>
       </c>
-      <c r="M1" s="88">
+      <c r="M1" s="87">
         <v>10</v>
       </c>
-      <c r="N1" s="88">
+      <c r="N1" s="87">
         <v>11</v>
       </c>
-      <c r="O1" s="88">
+      <c r="O1" s="87">
         <v>12</v>
       </c>
-      <c r="P1" s="88">
+      <c r="P1" s="87">
         <v>13</v>
       </c>
-      <c r="Q1" s="88">
+      <c r="Q1" s="87">
         <v>14</v>
       </c>
-      <c r="R1" s="88">
+      <c r="R1" s="87">
         <v>15</v>
       </c>
-      <c r="S1" s="88">
+      <c r="S1" s="87">
         <v>16</v>
       </c>
-      <c r="T1" s="88">
+      <c r="T1" s="87">
         <v>17</v>
       </c>
-      <c r="U1" s="88">
+      <c r="U1" s="87">
         <v>18</v>
       </c>
-      <c r="V1" s="88">
+      <c r="V1" s="87">
         <v>19</v>
       </c>
-      <c r="W1" s="88">
+      <c r="W1" s="87">
         <v>20</v>
       </c>
-      <c r="X1" s="88">
+      <c r="X1" s="87">
         <v>21</v>
       </c>
-      <c r="Y1" s="88">
+      <c r="Y1" s="87">
         <v>22</v>
       </c>
-      <c r="Z1" s="88">
+      <c r="Z1" s="87">
         <v>23</v>
       </c>
-      <c r="AA1" s="88">
+      <c r="AA1" s="87">
         <v>24</v>
       </c>
-      <c r="AB1" s="88">
+      <c r="AB1" s="87">
         <v>25</v>
       </c>
-      <c r="AC1" s="88">
+      <c r="AC1" s="87">
         <v>26</v>
       </c>
-      <c r="AD1" s="88">
+      <c r="AD1" s="87">
         <v>27</v>
       </c>
-      <c r="AE1" s="88">
+      <c r="AE1" s="87">
         <v>28</v>
       </c>
-      <c r="AF1" s="88">
+      <c r="AF1" s="87">
         <v>29</v>
       </c>
-      <c r="AG1" s="88">
+      <c r="AG1" s="87">
         <v>30</v>
       </c>
-      <c r="AH1" s="88">
+      <c r="AH1" s="87">
         <v>31</v>
       </c>
-      <c r="AI1" s="90" t="s">
+      <c r="AI1" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AJ1" s="91" t="s">
+      <c r="AJ1" s="90" t="s">
         <v>15</v>
       </c>
     </row>
@@ -35314,13 +35319,13 @@
       <c r="A2" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="91" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
       <c r="J2" s="41"/>
@@ -35348,11 +35353,11 @@
       <c r="AF2" s="41"/>
       <c r="AG2" s="41"/>
       <c r="AH2" s="41"/>
-      <c r="AI2" s="90">
+      <c r="AI2" s="89">
         <f>SUM(F2:AH2)</f>
         <v>0</v>
       </c>
-      <c r="AJ2" s="91" t="e">
+      <c r="AJ2" s="90" t="e">
         <f>AVERAGE(F2:AH2)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35361,28 +35366,28 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="K3" s="101" t="s">
+      <c r="K3" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="102"/>
-      <c r="M3" s="102"/>
-      <c r="N3" s="102"/>
-      <c r="O3" s="102"/>
-      <c r="P3" s="102"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="91" t="e">
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="108"/>
+      <c r="R3" s="90" t="e">
         <f>AVERAGE(D2:R2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB3" s="101" t="s">
+      <c r="AB3" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="102"/>
-      <c r="AD3" s="102"/>
-      <c r="AE3" s="102"/>
-      <c r="AF3" s="102"/>
-      <c r="AG3" s="107"/>
-      <c r="AH3" s="91" t="e">
+      <c r="AC3" s="103"/>
+      <c r="AD3" s="103"/>
+      <c r="AE3" s="103"/>
+      <c r="AF3" s="103"/>
+      <c r="AG3" s="108"/>
+      <c r="AH3" s="90" t="e">
         <f>AVERAGE(S2:AH2)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35393,115 +35398,115 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C5" s="87" t="s">
+      <c r="C5" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="88">
+      <c r="D5" s="87">
         <v>1</v>
       </c>
-      <c r="E5" s="88">
+      <c r="E5" s="87">
         <v>2</v>
       </c>
-      <c r="F5" s="89">
+      <c r="F5" s="88">
         <v>3</v>
       </c>
-      <c r="G5" s="88">
+      <c r="G5" s="87">
         <v>4</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="87">
         <v>5</v>
       </c>
-      <c r="I5" s="88">
+      <c r="I5" s="87">
         <v>6</v>
       </c>
-      <c r="J5" s="88">
+      <c r="J5" s="87">
         <v>7</v>
       </c>
-      <c r="K5" s="88">
+      <c r="K5" s="87">
         <v>8</v>
       </c>
-      <c r="L5" s="88">
+      <c r="L5" s="87">
         <v>9</v>
       </c>
-      <c r="M5" s="88">
+      <c r="M5" s="87">
         <v>10</v>
       </c>
-      <c r="N5" s="88">
+      <c r="N5" s="87">
         <v>11</v>
       </c>
-      <c r="O5" s="88">
+      <c r="O5" s="87">
         <v>12</v>
       </c>
-      <c r="P5" s="88">
+      <c r="P5" s="87">
         <v>13</v>
       </c>
-      <c r="Q5" s="88">
+      <c r="Q5" s="87">
         <v>14</v>
       </c>
-      <c r="R5" s="88">
+      <c r="R5" s="87">
         <v>15</v>
       </c>
-      <c r="S5" s="88">
+      <c r="S5" s="87">
         <v>16</v>
       </c>
-      <c r="T5" s="88">
+      <c r="T5" s="87">
         <v>17</v>
       </c>
-      <c r="U5" s="88">
+      <c r="U5" s="87">
         <v>18</v>
       </c>
-      <c r="V5" s="88">
+      <c r="V5" s="87">
         <v>19</v>
       </c>
-      <c r="W5" s="88">
+      <c r="W5" s="87">
         <v>20</v>
       </c>
-      <c r="X5" s="88">
+      <c r="X5" s="87">
         <v>21</v>
       </c>
-      <c r="Y5" s="88">
+      <c r="Y5" s="87">
         <v>22</v>
       </c>
-      <c r="Z5" s="88">
+      <c r="Z5" s="87">
         <v>23</v>
       </c>
-      <c r="AA5" s="88">
+      <c r="AA5" s="87">
         <v>24</v>
       </c>
-      <c r="AB5" s="88">
+      <c r="AB5" s="87">
         <v>25</v>
       </c>
-      <c r="AC5" s="88">
+      <c r="AC5" s="87">
         <v>26</v>
       </c>
-      <c r="AD5" s="88">
+      <c r="AD5" s="87">
         <v>27</v>
       </c>
-      <c r="AE5" s="88">
+      <c r="AE5" s="87">
         <v>28</v>
       </c>
-      <c r="AF5" s="88">
+      <c r="AF5" s="87">
         <v>29</v>
       </c>
-      <c r="AG5" s="88">
+      <c r="AG5" s="87">
         <v>30</v>
       </c>
-      <c r="AH5" s="93">
+      <c r="AH5" s="92">
         <v>31</v>
       </c>
-      <c r="AI5" s="90" t="s">
+      <c r="AI5" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AJ5" s="91" t="s">
+      <c r="AJ5" s="90" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
       <c r="H6" s="41"/>
@@ -35530,12 +35535,12 @@
       <c r="AE6" s="41"/>
       <c r="AF6" s="41"/>
       <c r="AG6" s="41"/>
-      <c r="AH6" s="94"/>
-      <c r="AI6" s="90">
+      <c r="AH6" s="93"/>
+      <c r="AI6" s="89">
         <f>SUM(D6:AH6)</f>
         <v>0</v>
       </c>
-      <c r="AJ6" s="91" t="e">
+      <c r="AJ6" s="90" t="e">
         <f>AVERAGE(F6:AH6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35544,28 +35549,28 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="K7" s="101" t="s">
+      <c r="K7" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="102"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="102"/>
-      <c r="O7" s="102"/>
-      <c r="P7" s="102"/>
-      <c r="Q7" s="107"/>
-      <c r="R7" s="91" t="e">
+      <c r="L7" s="103"/>
+      <c r="M7" s="103"/>
+      <c r="N7" s="103"/>
+      <c r="O7" s="103"/>
+      <c r="P7" s="103"/>
+      <c r="Q7" s="108"/>
+      <c r="R7" s="90" t="e">
         <f>AVERAGE(D6:R6)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB7" s="101" t="s">
+      <c r="AB7" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="102"/>
-      <c r="AD7" s="102"/>
-      <c r="AE7" s="102"/>
-      <c r="AF7" s="102"/>
-      <c r="AG7" s="107"/>
-      <c r="AH7" s="91" t="e">
+      <c r="AC7" s="103"/>
+      <c r="AD7" s="103"/>
+      <c r="AE7" s="103"/>
+      <c r="AF7" s="103"/>
+      <c r="AG7" s="108"/>
+      <c r="AH7" s="90" t="e">
         <f>AVERAGE(S6:AG6)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35576,115 +35581,115 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="88">
+      <c r="D9" s="87">
         <v>1</v>
       </c>
-      <c r="E9" s="88">
+      <c r="E9" s="87">
         <v>2</v>
       </c>
-      <c r="F9" s="89">
+      <c r="F9" s="88">
         <v>3</v>
       </c>
-      <c r="G9" s="88">
+      <c r="G9" s="87">
         <v>4</v>
       </c>
-      <c r="H9" s="88">
+      <c r="H9" s="87">
         <v>5</v>
       </c>
-      <c r="I9" s="88">
+      <c r="I9" s="87">
         <v>6</v>
       </c>
-      <c r="J9" s="88">
+      <c r="J9" s="87">
         <v>7</v>
       </c>
-      <c r="K9" s="88">
+      <c r="K9" s="87">
         <v>8</v>
       </c>
-      <c r="L9" s="88">
+      <c r="L9" s="87">
         <v>9</v>
       </c>
-      <c r="M9" s="88">
+      <c r="M9" s="87">
         <v>10</v>
       </c>
-      <c r="N9" s="88">
+      <c r="N9" s="87">
         <v>11</v>
       </c>
-      <c r="O9" s="88">
+      <c r="O9" s="87">
         <v>12</v>
       </c>
-      <c r="P9" s="88">
+      <c r="P9" s="87">
         <v>13</v>
       </c>
-      <c r="Q9" s="88">
+      <c r="Q9" s="87">
         <v>14</v>
       </c>
-      <c r="R9" s="88">
+      <c r="R9" s="87">
         <v>15</v>
       </c>
-      <c r="S9" s="88">
+      <c r="S9" s="87">
         <v>16</v>
       </c>
-      <c r="T9" s="88">
+      <c r="T9" s="87">
         <v>17</v>
       </c>
-      <c r="U9" s="88">
+      <c r="U9" s="87">
         <v>18</v>
       </c>
-      <c r="V9" s="88">
+      <c r="V9" s="87">
         <v>19</v>
       </c>
-      <c r="W9" s="88">
+      <c r="W9" s="87">
         <v>20</v>
       </c>
-      <c r="X9" s="88">
+      <c r="X9" s="87">
         <v>21</v>
       </c>
-      <c r="Y9" s="88">
+      <c r="Y9" s="87">
         <v>22</v>
       </c>
-      <c r="Z9" s="88">
+      <c r="Z9" s="87">
         <v>23</v>
       </c>
-      <c r="AA9" s="88">
+      <c r="AA9" s="87">
         <v>24</v>
       </c>
-      <c r="AB9" s="88">
+      <c r="AB9" s="87">
         <v>25</v>
       </c>
-      <c r="AC9" s="88">
+      <c r="AC9" s="87">
         <v>26</v>
       </c>
-      <c r="AD9" s="88">
+      <c r="AD9" s="87">
         <v>27</v>
       </c>
-      <c r="AE9" s="88">
+      <c r="AE9" s="87">
         <v>28</v>
       </c>
-      <c r="AF9" s="88">
+      <c r="AF9" s="87">
         <v>29</v>
       </c>
-      <c r="AG9" s="88">
+      <c r="AG9" s="87">
         <v>30</v>
       </c>
-      <c r="AH9" s="88">
+      <c r="AH9" s="87">
         <v>31</v>
       </c>
-      <c r="AI9" s="90" t="s">
+      <c r="AI9" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="AJ9" s="91" t="s">
+      <c r="AJ9" s="90" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
       <c r="F10" s="41"/>
       <c r="G10" s="41"/>
       <c r="H10" s="41"/>
@@ -35714,11 +35719,11 @@
       <c r="AF10" s="41"/>
       <c r="AG10" s="41"/>
       <c r="AH10" s="41"/>
-      <c r="AI10" s="90">
+      <c r="AI10" s="89">
         <f>SUM(D10:AH10)</f>
         <v>0</v>
       </c>
-      <c r="AJ10" s="91" t="e">
+      <c r="AJ10" s="90" t="e">
         <f>AVERAGE(F10:AH10)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35727,28 +35732,28 @@
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
-      <c r="K11" s="101" t="s">
+      <c r="K11" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="102"/>
-      <c r="M11" s="102"/>
-      <c r="N11" s="102"/>
-      <c r="O11" s="102"/>
-      <c r="P11" s="102"/>
-      <c r="Q11" s="107"/>
-      <c r="R11" s="91" t="e">
+      <c r="L11" s="103"/>
+      <c r="M11" s="103"/>
+      <c r="N11" s="103"/>
+      <c r="O11" s="103"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="108"/>
+      <c r="R11" s="90" t="e">
         <f>AVERAGE(D10:R10)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AB11" s="101" t="s">
+      <c r="AB11" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="AC11" s="102"/>
-      <c r="AD11" s="102"/>
-      <c r="AE11" s="102"/>
-      <c r="AF11" s="102"/>
-      <c r="AG11" s="107"/>
-      <c r="AH11" s="91" t="e">
+      <c r="AC11" s="103"/>
+      <c r="AD11" s="103"/>
+      <c r="AE11" s="103"/>
+      <c r="AF11" s="103"/>
+      <c r="AG11" s="108"/>
+      <c r="AH11" s="90" t="e">
         <f>AVERAGE(S10:AH10)</f>
         <v>#DIV/0!</v>
       </c>
@@ -35769,18 +35774,18 @@
       <c r="A13" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="67">
-        <v>8.2954E-2</v>
+      <c r="B13" s="98">
+        <v>7.3005E-2</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="69">
+      <c r="B14" s="68">
         <f>(B12*B13)</f>
         <v>0</v>
       </c>
@@ -35789,10 +35794,10 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="70">
+      <c r="B15" s="69">
         <f>B14/B22</f>
         <v>0</v>
       </c>
@@ -35804,52 +35809,52 @@
       <c r="A16" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="97">
+      <c r="B16" s="96">
         <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A17" s="68" t="s">
+      <c r="A17" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="69">
+      <c r="B17" s="68">
         <f>(B14*B16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A18" s="71"/>
-      <c r="B18" s="72"/>
+      <c r="A18" s="70"/>
+      <c r="B18" s="71"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="73" t="s">
+      <c r="A19" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="75">
+      <c r="B19" s="74">
         <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="73" t="s">
+      <c r="A20" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="75" t="e">
+      <c r="B20" s="74" t="e">
         <f>B19/(AJ2*B13)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="71"/>
-      <c r="B21" s="72"/>
+      <c r="A21" s="70"/>
+      <c r="B21" s="71"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A22" s="95" t="s">
+      <c r="A22" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="76">
-        <v>3585.49</v>
+      <c r="B22" s="75">
+        <v>3580.14</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -36876,7 +36881,7 @@
   <dimension ref="A1:AJ1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -36913,7 +36918,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="14.25" customHeight="1">
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="76" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="31">
@@ -37020,14 +37025,14 @@
       <c r="A2" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79" t="s">
+      <c r="B2" s="77"/>
+      <c r="C2" s="78" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="41"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
       <c r="H2" s="41"/>
       <c r="I2" s="41"/>
       <c r="J2" s="41"/>
@@ -37073,15 +37078,15 @@
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
-      <c r="K3" s="98" t="s">
+      <c r="K3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="99"/>
-      <c r="M3" s="99"/>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="100"/>
+      <c r="N3" s="100"/>
+      <c r="O3" s="100"/>
+      <c r="P3" s="100"/>
+      <c r="Q3" s="101"/>
       <c r="R3" s="48" t="e">
         <f>AVERAGE(D2:R2)</f>
         <v>#DIV/0!</v>
@@ -37095,14 +37100,14 @@
       <c r="Y3" s="47"/>
       <c r="Z3" s="47"/>
       <c r="AA3" s="47"/>
-      <c r="AB3" s="98" t="s">
+      <c r="AB3" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC3" s="99"/>
-      <c r="AD3" s="99"/>
-      <c r="AE3" s="99"/>
-      <c r="AF3" s="99"/>
-      <c r="AG3" s="100"/>
+      <c r="AC3" s="100"/>
+      <c r="AD3" s="100"/>
+      <c r="AE3" s="100"/>
+      <c r="AF3" s="100"/>
+      <c r="AG3" s="101"/>
       <c r="AH3" s="48" t="e">
         <f>AVERAGE(S2:AH2)</f>
         <v>#DIV/0!</v>
@@ -37119,14 +37124,14 @@
       <c r="H4" s="47"/>
       <c r="I4" s="47"/>
       <c r="J4" s="47"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="81"/>
+      <c r="K4" s="80"/>
+      <c r="L4" s="80"/>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="80"/>
       <c r="S4" s="47"/>
       <c r="T4" s="47"/>
       <c r="U4" s="47"/>
@@ -37136,7 +37141,7 @@
       <c r="Y4" s="47"/>
       <c r="Z4" s="47"/>
       <c r="AA4" s="47"/>
-      <c r="AB4" s="81"/>
+      <c r="AB4" s="80"/>
       <c r="AC4" s="47"/>
       <c r="AD4" s="47"/>
       <c r="AE4" s="47"/>
@@ -37234,13 +37239,13 @@
       <c r="AE5" s="52">
         <v>28</v>
       </c>
-      <c r="AF5" s="82">
+      <c r="AF5" s="81">
         <v>29</v>
       </c>
-      <c r="AG5" s="82">
+      <c r="AG5" s="81">
         <v>30</v>
       </c>
-      <c r="AH5" s="82">
+      <c r="AH5" s="81">
         <v>31</v>
       </c>
       <c r="AI5" s="43" t="s">
@@ -37303,15 +37308,15 @@
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
       <c r="J7" s="47"/>
-      <c r="K7" s="98" t="s">
+      <c r="K7" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="99"/>
-      <c r="M7" s="99"/>
-      <c r="N7" s="99"/>
-      <c r="O7" s="99"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="100"/>
+      <c r="L7" s="100"/>
+      <c r="M7" s="100"/>
+      <c r="N7" s="100"/>
+      <c r="O7" s="100"/>
+      <c r="P7" s="100"/>
+      <c r="Q7" s="101"/>
       <c r="R7" s="48" t="e">
         <f>AVERAGE(D6:R6)</f>
         <v>#DIV/0!</v>
@@ -37325,14 +37330,14 @@
       <c r="Y7" s="47"/>
       <c r="Z7" s="47"/>
       <c r="AA7" s="47"/>
-      <c r="AB7" s="98" t="s">
+      <c r="AB7" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC7" s="99"/>
-      <c r="AD7" s="99"/>
-      <c r="AE7" s="99"/>
-      <c r="AF7" s="99"/>
-      <c r="AG7" s="100"/>
+      <c r="AC7" s="100"/>
+      <c r="AD7" s="100"/>
+      <c r="AE7" s="100"/>
+      <c r="AF7" s="100"/>
+      <c r="AG7" s="101"/>
       <c r="AH7" s="48" t="e">
         <f>AVERAGE(S6:AE6)</f>
         <v>#DIV/0!</v>
@@ -37491,8 +37496,8 @@
       <c r="A10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="67">
-        <v>8.2954E-2</v>
+      <c r="B10" s="98">
+        <v>7.3005E-2</v>
       </c>
       <c r="C10" s="36" t="s">
         <v>4</v>
@@ -37538,10 +37543,10 @@
       </c>
     </row>
     <row r="11" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="68">
         <f>(B9*B10)</f>
         <v>0</v>
       </c>
@@ -37553,15 +37558,15 @@
       <c r="H11" s="47"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
-      <c r="K11" s="98" t="s">
+      <c r="K11" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="99"/>
-      <c r="M11" s="99"/>
-      <c r="N11" s="99"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="100"/>
+      <c r="L11" s="100"/>
+      <c r="M11" s="100"/>
+      <c r="N11" s="100"/>
+      <c r="O11" s="100"/>
+      <c r="P11" s="100"/>
+      <c r="Q11" s="101"/>
       <c r="R11" s="48" t="e">
         <f>AVERAGE(D10:R10)</f>
         <v>#DIV/0!</v>
@@ -37575,14 +37580,14 @@
       <c r="Y11" s="47"/>
       <c r="Z11" s="47"/>
       <c r="AA11" s="47"/>
-      <c r="AB11" s="98" t="s">
+      <c r="AB11" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC11" s="99"/>
-      <c r="AD11" s="99"/>
-      <c r="AE11" s="99"/>
-      <c r="AF11" s="99"/>
-      <c r="AG11" s="100"/>
+      <c r="AC11" s="100"/>
+      <c r="AD11" s="100"/>
+      <c r="AE11" s="100"/>
+      <c r="AF11" s="100"/>
+      <c r="AG11" s="101"/>
       <c r="AH11" s="48" t="e">
         <f>AVERAGE(S10:AH10)</f>
         <v>#DIV/0!</v>
@@ -37591,10 +37596,10 @@
       <c r="AJ11" s="49"/>
     </row>
     <row r="12" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="70">
+      <c r="B12" s="69">
         <f>B11/B16</f>
         <v>0</v>
       </c>
@@ -37637,7 +37642,7 @@
       <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="97">
+      <c r="B13" s="96">
         <v>185</v>
       </c>
       <c r="C13" s="50" t="s">
@@ -37733,7 +37738,7 @@
       <c r="AG13" s="52">
         <v>30</v>
       </c>
-      <c r="AH13" s="82">
+      <c r="AH13" s="81">
         <v>31</v>
       </c>
       <c r="AI13" s="43" t="s">
@@ -37744,10 +37749,10 @@
       </c>
     </row>
     <row r="14" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="69">
+      <c r="B14" s="68">
         <f>(B11*B13)</f>
         <v>0</v>
       </c>
@@ -37795,8 +37800,8 @@
       </c>
     </row>
     <row r="15" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A15" s="71"/>
-      <c r="B15" s="72"/>
+      <c r="A15" s="70"/>
+      <c r="B15" s="71"/>
       <c r="C15" s="45"/>
       <c r="D15" s="46"/>
       <c r="E15" s="46"/>
@@ -37805,15 +37810,15 @@
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47"/>
-      <c r="K15" s="98" t="s">
+      <c r="K15" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="99"/>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="100"/>
+      <c r="L15" s="100"/>
+      <c r="M15" s="100"/>
+      <c r="N15" s="100"/>
+      <c r="O15" s="100"/>
+      <c r="P15" s="100"/>
+      <c r="Q15" s="101"/>
       <c r="R15" s="48" t="e">
         <f>AVERAGE(D14:R14)</f>
         <v>#DIV/0!</v>
@@ -37827,14 +37832,14 @@
       <c r="Y15" s="47"/>
       <c r="Z15" s="47"/>
       <c r="AA15" s="47"/>
-      <c r="AB15" s="98" t="s">
+      <c r="AB15" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC15" s="99"/>
-      <c r="AD15" s="99"/>
-      <c r="AE15" s="99"/>
-      <c r="AF15" s="99"/>
-      <c r="AG15" s="100"/>
+      <c r="AC15" s="100"/>
+      <c r="AD15" s="100"/>
+      <c r="AE15" s="100"/>
+      <c r="AF15" s="100"/>
+      <c r="AG15" s="101"/>
       <c r="AH15" s="48" t="e">
         <f>AVERAGE(S14:AG14)</f>
         <v>#DIV/0!</v>
@@ -37843,11 +37848,11 @@
       <c r="AJ15" s="49"/>
     </row>
     <row r="16" spans="1:36" ht="14.25" customHeight="1">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="76">
-        <v>3585.49</v>
+      <c r="B16" s="75">
+        <v>3580.14</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="46"/>
@@ -38041,15 +38046,15 @@
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="47"/>
-      <c r="K19" s="98" t="s">
+      <c r="K19" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L19" s="99"/>
-      <c r="M19" s="99"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="100"/>
+      <c r="L19" s="100"/>
+      <c r="M19" s="100"/>
+      <c r="N19" s="100"/>
+      <c r="O19" s="100"/>
+      <c r="P19" s="100"/>
+      <c r="Q19" s="101"/>
       <c r="R19" s="48" t="e">
         <f>AVERAGE(D18:R18)</f>
         <v>#DIV/0!</v>
@@ -38063,14 +38068,14 @@
       <c r="Y19" s="47"/>
       <c r="Z19" s="47"/>
       <c r="AA19" s="47"/>
-      <c r="AB19" s="98" t="s">
+      <c r="AB19" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC19" s="99"/>
-      <c r="AD19" s="99"/>
-      <c r="AE19" s="99"/>
-      <c r="AF19" s="99"/>
-      <c r="AG19" s="100"/>
+      <c r="AC19" s="100"/>
+      <c r="AD19" s="100"/>
+      <c r="AE19" s="100"/>
+      <c r="AF19" s="100"/>
+      <c r="AG19" s="101"/>
       <c r="AH19" s="48" t="e">
         <f>AVERAGE(S18:AG18)</f>
         <v>#DIV/0!</v>
@@ -38208,7 +38213,7 @@
       <c r="AG21" s="52">
         <v>30</v>
       </c>
-      <c r="AH21" s="82">
+      <c r="AH21" s="81">
         <v>31</v>
       </c>
       <c r="AI21" s="43" t="s">
@@ -38271,15 +38276,15 @@
       <c r="H23" s="47"/>
       <c r="I23" s="47"/>
       <c r="J23" s="47"/>
-      <c r="K23" s="98" t="s">
+      <c r="K23" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L23" s="99"/>
-      <c r="M23" s="99"/>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+      <c r="N23" s="100"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="100"/>
+      <c r="Q23" s="101"/>
       <c r="R23" s="48" t="e">
         <f>AVERAGE(D22:R22)</f>
         <v>#DIV/0!</v>
@@ -38293,14 +38298,14 @@
       <c r="Y23" s="47"/>
       <c r="Z23" s="47"/>
       <c r="AA23" s="47"/>
-      <c r="AB23" s="98" t="s">
+      <c r="AB23" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC23" s="99"/>
-      <c r="AD23" s="99"/>
-      <c r="AE23" s="99"/>
-      <c r="AF23" s="99"/>
-      <c r="AG23" s="100"/>
+      <c r="AC23" s="100"/>
+      <c r="AD23" s="100"/>
+      <c r="AE23" s="100"/>
+      <c r="AF23" s="100"/>
+      <c r="AG23" s="101"/>
       <c r="AH23" s="48" t="e">
         <f>AVERAGE(S22:AG22)</f>
         <v>#DIV/0!</v>
@@ -38501,36 +38506,36 @@
       <c r="H27" s="47"/>
       <c r="I27" s="47"/>
       <c r="J27" s="47"/>
-      <c r="K27" s="98" t="s">
+      <c r="K27" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L27" s="99"/>
-      <c r="M27" s="99"/>
-      <c r="N27" s="99"/>
-      <c r="O27" s="99"/>
-      <c r="P27" s="99"/>
-      <c r="Q27" s="100"/>
+      <c r="L27" s="100"/>
+      <c r="M27" s="100"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="100"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="101"/>
       <c r="R27" s="48" t="e">
         <f>AVERAGE(D26:R26)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S27" s="83"/>
-      <c r="T27" s="83"/>
-      <c r="U27" s="83"/>
-      <c r="V27" s="84"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="83"/>
       <c r="W27" s="47"/>
       <c r="X27" s="47"/>
       <c r="Y27" s="47"/>
       <c r="Z27" s="47"/>
       <c r="AA27" s="47"/>
-      <c r="AB27" s="98" t="s">
+      <c r="AB27" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC27" s="99"/>
-      <c r="AD27" s="99"/>
-      <c r="AE27" s="99"/>
-      <c r="AF27" s="99"/>
-      <c r="AG27" s="100"/>
+      <c r="AC27" s="100"/>
+      <c r="AD27" s="100"/>
+      <c r="AE27" s="100"/>
+      <c r="AF27" s="100"/>
+      <c r="AG27" s="101"/>
       <c r="AH27" s="48" t="e">
         <f>AVERAGE(S26:AH26)</f>
         <v>#DIV/0!</v>
@@ -38731,15 +38736,15 @@
       <c r="H31" s="47"/>
       <c r="I31" s="47"/>
       <c r="J31" s="47"/>
-      <c r="K31" s="98" t="s">
+      <c r="K31" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L31" s="99"/>
-      <c r="M31" s="99"/>
-      <c r="N31" s="99"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="100"/>
+      <c r="L31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="101"/>
       <c r="R31" s="48" t="e">
         <f>AVERAGE(D30:R30)</f>
         <v>#DIV/0!</v>
@@ -38753,14 +38758,14 @@
       <c r="Y31" s="47"/>
       <c r="Z31" s="47"/>
       <c r="AA31" s="47"/>
-      <c r="AB31" s="98" t="s">
+      <c r="AB31" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC31" s="99"/>
-      <c r="AD31" s="99"/>
-      <c r="AE31" s="99"/>
-      <c r="AF31" s="99"/>
-      <c r="AG31" s="100"/>
+      <c r="AC31" s="100"/>
+      <c r="AD31" s="100"/>
+      <c r="AE31" s="100"/>
+      <c r="AF31" s="100"/>
+      <c r="AG31" s="101"/>
       <c r="AH31" s="48" t="e">
         <f>AVERAGE(S30:AH30)</f>
         <v>#DIV/0!</v>
@@ -38898,7 +38903,7 @@
       <c r="AG33" s="52">
         <v>30</v>
       </c>
-      <c r="AH33" s="82">
+      <c r="AH33" s="81">
         <v>31</v>
       </c>
       <c r="AI33" s="43" t="s">
@@ -38953,7 +38958,7 @@
       </c>
     </row>
     <row r="35" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C35" s="85"/>
+      <c r="C35" s="84"/>
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
       <c r="F35" s="47"/>
@@ -38961,15 +38966,15 @@
       <c r="H35" s="47"/>
       <c r="I35" s="47"/>
       <c r="J35" s="47"/>
-      <c r="K35" s="98" t="s">
+      <c r="K35" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L35" s="99"/>
-      <c r="M35" s="99"/>
-      <c r="N35" s="99"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="100"/>
+      <c r="L35" s="100"/>
+      <c r="M35" s="100"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="100"/>
+      <c r="P35" s="100"/>
+      <c r="Q35" s="101"/>
       <c r="R35" s="48" t="e">
         <f>AVERAGE(D34:R34)</f>
         <v>#DIV/0!</v>
@@ -38983,14 +38988,14 @@
       <c r="Y35" s="47"/>
       <c r="Z35" s="47"/>
       <c r="AA35" s="47"/>
-      <c r="AB35" s="98" t="s">
+      <c r="AB35" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC35" s="99"/>
-      <c r="AD35" s="99"/>
-      <c r="AE35" s="99"/>
-      <c r="AF35" s="99"/>
-      <c r="AG35" s="100"/>
+      <c r="AC35" s="100"/>
+      <c r="AD35" s="100"/>
+      <c r="AE35" s="100"/>
+      <c r="AF35" s="100"/>
+      <c r="AG35" s="101"/>
       <c r="AH35" s="48" t="e">
         <f>AVERAGE(S34:AG34)</f>
         <v>#DIV/0!</v>
@@ -38999,7 +39004,7 @@
       <c r="AJ35" s="49"/>
     </row>
     <row r="36" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C36" s="85"/>
+      <c r="C36" s="84"/>
       <c r="D36" s="47"/>
       <c r="E36" s="47"/>
       <c r="F36" s="47"/>
@@ -39191,15 +39196,15 @@
       <c r="H39" s="47"/>
       <c r="I39" s="47"/>
       <c r="J39" s="47"/>
-      <c r="K39" s="98" t="s">
+      <c r="K39" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L39" s="99"/>
-      <c r="M39" s="99"/>
-      <c r="N39" s="99"/>
-      <c r="O39" s="99"/>
-      <c r="P39" s="99"/>
-      <c r="Q39" s="100"/>
+      <c r="L39" s="100"/>
+      <c r="M39" s="100"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="100"/>
+      <c r="Q39" s="101"/>
       <c r="R39" s="48" t="e">
         <f>AVERAGE(D38:R38)</f>
         <v>#DIV/0!</v>
@@ -39213,14 +39218,14 @@
       <c r="Y39" s="47"/>
       <c r="Z39" s="47"/>
       <c r="AA39" s="47"/>
-      <c r="AB39" s="98" t="s">
+      <c r="AB39" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC39" s="99"/>
-      <c r="AD39" s="99"/>
-      <c r="AE39" s="99"/>
-      <c r="AF39" s="99"/>
-      <c r="AG39" s="100"/>
+      <c r="AC39" s="100"/>
+      <c r="AD39" s="100"/>
+      <c r="AE39" s="100"/>
+      <c r="AF39" s="100"/>
+      <c r="AG39" s="101"/>
       <c r="AH39" s="48" t="e">
         <f>AVERAGE(S38:AH38)</f>
         <v>#DIV/0!</v>
@@ -39358,7 +39363,7 @@
       <c r="AG41" s="52">
         <v>30</v>
       </c>
-      <c r="AH41" s="82">
+      <c r="AH41" s="81">
         <v>31</v>
       </c>
       <c r="AI41" s="43" t="s">
@@ -39421,15 +39426,15 @@
       <c r="H43" s="47"/>
       <c r="I43" s="47"/>
       <c r="J43" s="47"/>
-      <c r="K43" s="98" t="s">
+      <c r="K43" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L43" s="99"/>
-      <c r="M43" s="99"/>
-      <c r="N43" s="99"/>
-      <c r="O43" s="99"/>
-      <c r="P43" s="99"/>
-      <c r="Q43" s="100"/>
+      <c r="L43" s="100"/>
+      <c r="M43" s="100"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="100"/>
+      <c r="Q43" s="101"/>
       <c r="R43" s="48" t="e">
         <f>AVERAGE(D42:R42)</f>
         <v>#DIV/0!</v>
@@ -39443,14 +39448,14 @@
       <c r="Y43" s="47"/>
       <c r="Z43" s="47"/>
       <c r="AA43" s="47"/>
-      <c r="AB43" s="98" t="s">
+      <c r="AB43" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="AC43" s="99"/>
-      <c r="AD43" s="99"/>
-      <c r="AE43" s="99"/>
-      <c r="AF43" s="99"/>
-      <c r="AG43" s="100"/>
+      <c r="AC43" s="100"/>
+      <c r="AD43" s="100"/>
+      <c r="AE43" s="100"/>
+      <c r="AF43" s="100"/>
+      <c r="AG43" s="101"/>
       <c r="AH43" s="48" t="e">
         <f>AVERAGE(S42:AG42)</f>
         <v>#DIV/0!</v>
@@ -39643,7 +39648,7 @@
       </c>
     </row>
     <row r="47" spans="3:36" ht="14.25" customHeight="1">
-      <c r="C47" s="86"/>
+      <c r="C47" s="85"/>
       <c r="D47" s="61"/>
       <c r="E47" s="61"/>
       <c r="F47" s="61"/>
@@ -39651,15 +39656,15 @@
       <c r="H47" s="61"/>
       <c r="I47" s="61"/>
       <c r="J47" s="61"/>
-      <c r="K47" s="104" t="s">
+      <c r="K47" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="L47" s="105"/>
-      <c r="M47" s="105"/>
-      <c r="N47" s="105"/>
-      <c r="O47" s="105"/>
-      <c r="P47" s="105"/>
-      <c r="Q47" s="106"/>
+      <c r="L47" s="106"/>
+      <c r="M47" s="106"/>
+      <c r="N47" s="106"/>
+      <c r="O47" s="106"/>
+      <c r="P47" s="106"/>
+      <c r="Q47" s="107"/>
       <c r="R47" s="62" t="e">
         <f>AVERAGE(D46:R46)</f>
         <v>#DIV/0!</v>
@@ -39673,14 +39678,14 @@
       <c r="Y47" s="61"/>
       <c r="Z47" s="61"/>
       <c r="AA47" s="61"/>
-      <c r="AB47" s="104" t="s">
+      <c r="AB47" s="105" t="s">
         <v>17</v>
       </c>
-      <c r="AC47" s="105"/>
-      <c r="AD47" s="105"/>
-      <c r="AE47" s="105"/>
-      <c r="AF47" s="105"/>
-      <c r="AG47" s="106"/>
+      <c r="AC47" s="106"/>
+      <c r="AD47" s="106"/>
+      <c r="AE47" s="106"/>
+      <c r="AF47" s="106"/>
+      <c r="AG47" s="107"/>
       <c r="AH47" s="62" t="e">
         <f>AVERAGE(S46:AH46)</f>
         <v>#DIV/0!</v>
@@ -40643,6 +40648,18 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="AB3:AG3"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="AB7:AG7"/>
+    <mergeCell ref="K11:Q11"/>
+    <mergeCell ref="AB11:AG11"/>
+    <mergeCell ref="AB15:AG15"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K19:Q19"/>
+    <mergeCell ref="AB19:AG19"/>
+    <mergeCell ref="K23:Q23"/>
+    <mergeCell ref="AB23:AG23"/>
     <mergeCell ref="K27:Q27"/>
     <mergeCell ref="AB27:AG27"/>
     <mergeCell ref="K43:Q43"/>
@@ -40655,18 +40672,6 @@
     <mergeCell ref="K39:Q39"/>
     <mergeCell ref="AB39:AG39"/>
     <mergeCell ref="AB43:AG43"/>
-    <mergeCell ref="AB15:AG15"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="K19:Q19"/>
-    <mergeCell ref="AB19:AG19"/>
-    <mergeCell ref="K23:Q23"/>
-    <mergeCell ref="AB23:AG23"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="AB3:AG3"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="AB7:AG7"/>
-    <mergeCell ref="K11:Q11"/>
-    <mergeCell ref="AB11:AG11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>